<commit_message>
Reduced bugs in parameter detection
Signed-off-by: Sajed Jalil <sjalil@gmu.edu>
</commit_message>
<xml_diff>
--- a/res/API-dictionary.xlsx
+++ b/res/API-dictionary.xlsx
@@ -1332,13 +1332,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B153" activeCellId="0" sqref="B153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.8"/>
@@ -2880,11 +2880,13 @@
         <v>397</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="0" t="s">
         <v>398</v>
       </c>
     </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>